<commit_message>
Update about and contact, show invalid ids
Signed-off-by: rtgdk <rohit.lodhartg@gmail.com>
</commit_message>
<xml_diff>
--- a/static/sample-sheet-grubs.xlsx
+++ b/static/sample-sheet-grubs.xlsx
@@ -5,49 +5,61 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>BITS ID</t>
-  </si>
-  <si>
-    <t>MEAL TYPE</t>
-  </si>
-  <si>
-    <t>Student Bits id</t>
-  </si>
-  <si>
-    <t>Veg or veg</t>
-  </si>
-  <si>
-    <t>Eg: 2010B3A2735P</t>
-  </si>
-  <si>
-    <t>Non Veg or non veg</t>
-  </si>
-  <si>
-    <t>Eg: 2010A1TS123P</t>
-  </si>
-  <si>
-    <t>Eg: 2006PH12559P</t>
-  </si>
-  <si>
-    <t>Eg: 2007PHXF424P</t>
-  </si>
-  <si>
-    <t>Order of First Row should not be changed.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t xml:space="preserve">BITS ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEAL TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student Bits id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veg or veg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eg: 2010B3A20735P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Veg or non veg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eg: 2010A1TS0123P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eg: 2006PH120559P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eg: 2007PHXF0424P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order of First Row should not be changed.</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Above rows (except 1</t>
     </r>
     <r>
@@ -73,10 +85,13 @@
     </r>
   </si>
   <si>
-    <t>All the fields should be valid.</t>
-  </si>
-  <si>
-    <t>Nothing Else should be written in any other column</t>
+    <t xml:space="preserve">All the fields should be valid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing Else should be written in any other column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don’t forget to add 0 before ID for 2016 or earler batch</t>
   </si>
 </sst>
 </file>
@@ -84,29 +99,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -114,17 +109,26 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -182,23 +186,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,17 +223,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,6 +309,11 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>